<commit_message>
modified:   5/5.py 	new file:   5/BDE.xlsx 	new file:   5/InformeAutomatico.xlsx
</commit_message>
<xml_diff>
--- a/5/Informes.xlsx
+++ b/5/Informes.xlsx
@@ -2,31 +2,43 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristopher\Desktop\De Todo\Universidad\LdL\BackEnd\Laboratorio-Full-\Back-End\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristopher\Desktop\De Todo\Universidad\LdL\BackEnd\5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475AFA14-EA80-4296-9B28-DE0FEAA597D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138D8080-F691-48CA-BFCC-438A88F4163A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8E26A613-0ACC-4FB8-A1EB-89332EFD880A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Primer Informe" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Cant. Total</t>
+    <t>Localidad</t>
   </si>
   <si>
-    <t>Dia</t>
+    <t>Servicio</t>
   </si>
   <si>
     <t>Total</t>
@@ -36,8 +48,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,14 +85,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,19 +177,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{990DF440-8868-43A7-BFB3-7AEBC47E54DC}" name="Tabla1" displayName="Tabla1" ref="A1:C17" totalsRowShown="0">
-  <autoFilter ref="A1:C17" xr:uid="{990DF440-8868-43A7-BFB3-7AEBC47E54DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{195DDFFD-594F-453D-B766-C04476FD73D3}" name="Tabla1" displayName="Tabla1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:C6" xr:uid="{195DDFFD-594F-453D-B766-C04476FD73D3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{77A44142-DA13-422C-942F-60481CE6F1E8}" name="Cant. Total"/>
-    <tableColumn id="2" xr3:uid="{053131C9-B2D4-47EC-80B1-C9DE83B8530F}" name="Dia"/>
-    <tableColumn id="3" xr3:uid="{8D4FDCEE-BDAB-47E6-BF5B-A65ADE7745DD}" name="Total"/>
+    <tableColumn id="1" xr3:uid="{104C0074-050F-46E0-8CF8-D886787B9ADF}" name="Localidad" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{103D4470-386A-410B-8104-CE5903F1493A}" name="Servicio" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{785EE4CD-515C-40F5-97D4-B19ACDC0676D}" name="Total" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -107,44 +199,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -171,14 +263,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -205,6 +315,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -216,210 +344,196 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CE8F44-01C5-42DD-AFD0-BB3B45CB97D3}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="12" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>